<commit_message>
feat: support bool and float scalar types, in-cell message type, rows and columns transpose
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Github/tableau/cmd/test/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC047D0A-EBA0-4640-AC4A-1DC7B3BA8D09}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055CC890-E12B-384C-8700-28175E3B8A0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2730" yWindow="3405" windowWidth="37020" windowHeight="13740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="2060" yWindow="880" windowWidth="28800" windowHeight="13740" activeTab="2" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
     <sheet name="Activity" sheetId="2" r:id="rId2"/>
+    <sheet name="Env" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>道具ID</t>
   </si>
@@ -227,6 +228,42 @@
   </si>
   <si>
     <t>1:50,2:900,3:2000</t>
+  </si>
+  <si>
+    <t>ZoneID</t>
+  </si>
+  <si>
+    <t>WorldID</t>
+  </si>
+  <si>
+    <t>PlatformType</t>
+  </si>
+  <si>
+    <t>赠送的道具</t>
+  </si>
+  <si>
+    <t>测试</t>
+  </si>
+  <si>
+    <t>1001:2,1002:5,1003:10</t>
+  </si>
+  <si>
+    <t>基本信息</t>
+  </si>
+  <si>
+    <t>110,标题,内容,true</t>
+  </si>
+  <si>
+    <t>比例</t>
+  </si>
+  <si>
+    <t>系数</t>
+  </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>15.246879</t>
   </si>
 </sst>
 </file>
@@ -268,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -279,9 +316,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -297,7 +340,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -595,32 +638,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.875" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="1"/>
-    <col min="5" max="5" width="10.875" style="2"/>
-    <col min="6" max="8" width="14.375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.625" style="2" customWidth="1"/>
-    <col min="10" max="11" width="14.375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.875" style="2"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="8" width="14.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" style="2" customWidth="1"/>
+    <col min="10" max="11" width="14.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="2"/>
     <col min="13" max="13" width="12.5" style="2" customWidth="1"/>
-    <col min="14" max="15" width="14.375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="19.625" style="2" customWidth="1"/>
-    <col min="17" max="18" width="14.375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="10.875" style="1"/>
+    <col min="14" max="15" width="14.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" style="2" customWidth="1"/>
+    <col min="17" max="18" width="14.33203125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="1"/>
     <col min="20" max="20" width="24.5" style="3" customWidth="1"/>
-    <col min="21" max="21" width="25.125" style="3" customWidth="1"/>
-    <col min="22" max="22" width="20.875" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.875" style="1"/>
+    <col min="21" max="21" width="25.1640625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="20.83203125" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +731,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
@@ -756,7 +799,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
@@ -824,7 +867,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1003</v>
       </c>
@@ -903,18 +946,18 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
     <col min="10" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="20.875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -952,7 +995,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>100001</v>
       </c>
@@ -990,7 +1033,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>100001</v>
       </c>
@@ -1028,7 +1071,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1066,7 +1109,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>100002</v>
       </c>
@@ -1104,7 +1147,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>100003</v>
       </c>
@@ -1140,6 +1183,89 @@
       </c>
       <c r="L6" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788C4DC7-4113-0642-9BB8-FA63AD1AD680}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: horizontal layout map
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Github/tableau/cmd/test/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055CC890-E12B-384C-8700-28175E3B8A0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B44217-563C-2E4C-AF4C-5C23FF134BDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="880" windowWidth="28800" windowHeight="13740" activeTab="2" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-1060" yWindow="3180" windowWidth="28800" windowHeight="13740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>道具ID</t>
   </si>
@@ -206,18 +206,6 @@
     <t>强化1描述3</t>
   </si>
   <si>
-    <t>属性1类型</t>
-  </si>
-  <si>
-    <t>属性1数量</t>
-  </si>
-  <si>
-    <t>属性2类型</t>
-  </si>
-  <si>
-    <t>属性2数量</t>
-  </si>
-  <si>
     <t>售卖选项</t>
   </si>
   <si>
@@ -264,6 +252,24 @@
   </si>
   <si>
     <t>15.246879</t>
+  </si>
+  <si>
+    <t>属性1抑制1类型</t>
+  </si>
+  <si>
+    <t>属性1抑制1数量</t>
+  </si>
+  <si>
+    <t>属性1抑制2类型</t>
+  </si>
+  <si>
+    <t>属性1抑制2数量</t>
+  </si>
+  <si>
+    <t>属性2抑制1类型</t>
+  </si>
+  <si>
+    <t>属性2抑制1数量</t>
   </si>
 </sst>
 </file>
@@ -636,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,20 +656,24 @@
     <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="6" max="8" width="14.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="19.6640625" style="2" customWidth="1"/>
-    <col min="10" max="11" width="14.33203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="2"/>
-    <col min="13" max="13" width="12.5" style="2" customWidth="1"/>
-    <col min="14" max="15" width="14.33203125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" style="2" customWidth="1"/>
-    <col min="17" max="18" width="14.33203125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" style="1"/>
-    <col min="20" max="20" width="24.5" style="3" customWidth="1"/>
-    <col min="21" max="21" width="25.1640625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="20.83203125" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="19.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="18.5" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="2"/>
+    <col min="15" max="15" width="12.5" style="2" customWidth="1"/>
+    <col min="16" max="17" width="14.33203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.6640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="17.83203125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" style="1"/>
+    <col min="22" max="22" width="24.5" style="3" customWidth="1"/>
+    <col min="23" max="23" width="25.1640625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="20.83203125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,46 +702,52 @@
         <v>43</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
@@ -766,40 +782,46 @@
         <v>1</v>
       </c>
       <c r="L2" s="2">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="2">
         <v>2002</v>
       </c>
-      <c r="M2" s="2">
-        <v>2</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
+        <v>2</v>
+      </c>
+      <c r="P2" s="2">
         <v>11</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2">
         <v>5</v>
       </c>
-      <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
@@ -834,40 +856,46 @@
         <v>1</v>
       </c>
       <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
         <v>2002</v>
       </c>
-      <c r="M3" s="2">
-        <v>2</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
+        <v>2</v>
+      </c>
+      <c r="P3" s="2">
         <v>12</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" s="2">
-        <v>2</v>
-      </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
+        <v>2</v>
+      </c>
+      <c r="T3" s="2">
         <v>6</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1003</v>
       </c>
@@ -902,36 +930,42 @@
         <v>1</v>
       </c>
       <c r="L4" s="2">
+        <v>3</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
         <v>2002</v>
       </c>
-      <c r="M4" s="2">
-        <v>2</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2">
         <v>13</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="S4" s="2">
         <v>3</v>
       </c>
-      <c r="R4" s="2">
+      <c r="T4" s="2">
         <v>7</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="T4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1194,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788C4DC7-4113-0642-9BB8-FA63AD1AD680}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1206,7 +1240,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
@@ -1214,7 +1248,7 @@
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
@@ -1222,7 +1256,7 @@
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -1233,39 +1267,39 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: custom captrow and datarow
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Github/tableau/cmd/test/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B44217-563C-2E4C-AF4C-5C23FF134BDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F370C8FD-F6AC-974A-B810-1D20B53D80EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1060" yWindow="3180" windowWidth="28800" windowHeight="13740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="1720" yWindow="2700" windowWidth="28800" windowHeight="13740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t>道具ID</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>属性2抑制1数量</t>
+  </si>
+  <si>
+    <t>descrow</t>
   </si>
 </sst>
 </file>
@@ -642,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,164 +678,164 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="W2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1001</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5001001</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2001</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2">
-        <v>2</v>
-      </c>
-      <c r="N2" s="2">
-        <v>2002</v>
-      </c>
-      <c r="O2" s="2">
-        <v>2</v>
-      </c>
-      <c r="P2" s="2">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S2" s="2">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2">
-        <v>5</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>5001002</v>
+        <v>5001001</v>
       </c>
       <c r="E3" s="2">
         <v>2001</v>
@@ -841,16 +844,16 @@
         <v>1</v>
       </c>
       <c r="G3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="2">
         <v>1</v>
@@ -859,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="M3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3" s="2">
         <v>2002</v>
@@ -868,25 +871,25 @@
         <v>2</v>
       </c>
       <c r="P3" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T3" s="2">
-        <v>6</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>4</v>
@@ -897,16 +900,16 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
-        <v>5001003</v>
+        <v>5001002</v>
       </c>
       <c r="E4" s="2">
         <v>2001</v>
@@ -915,22 +918,22 @@
         <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" s="2">
         <v>1</v>
       </c>
       <c r="L4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M4" s="2">
         <v>1</v>
@@ -942,30 +945,104 @@
         <v>2</v>
       </c>
       <c r="P4" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="S4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T4" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5001003</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>3</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2002</v>
+      </c>
+      <c r="O5" s="2">
+        <v>2</v>
+      </c>
+      <c r="P5" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="2">
+        <v>3</v>
+      </c>
+      <c r="T5" s="2">
+        <v>7</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" s="3" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: duration in the form
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Github/tableau/cmd/test/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C49962-377C-864E-8926-62DBF3D294DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD84106-3BD4-414C-9190-EAEFE63E94A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2700" windowWidth="28800" windowHeight="13740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-435" yWindow="5625" windowWidth="37020" windowHeight="13740" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
   <si>
     <t>道具ID</t>
   </si>
@@ -152,9 +152,6 @@
     <t>有效多久</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>持续多久</t>
   </si>
   <si>
@@ -270,6 +267,21 @@
   </si>
   <si>
     <t>descrow</t>
+  </si>
+  <si>
+    <t>72h3m0.5s</t>
+  </si>
+  <si>
+    <t>1m0.5s</t>
+  </si>
+  <si>
+    <t>1h1s</t>
+  </si>
+  <si>
+    <t>1h1m</t>
+  </si>
+  <si>
+    <t>1h1m1s</t>
   </si>
 </sst>
 </file>
@@ -330,7 +342,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -346,7 +358,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -644,110 +656,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:X5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.875" style="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="8" width="14.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="1"/>
+    <col min="5" max="5" width="10.875" style="2"/>
+    <col min="6" max="8" width="14.375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="18.625" style="2" customWidth="1"/>
     <col min="13" max="13" width="18.5" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="10.875" style="2"/>
     <col min="15" max="15" width="12.5" style="2" customWidth="1"/>
-    <col min="16" max="17" width="14.33203125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="17.83203125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" style="1"/>
+    <col min="16" max="17" width="14.375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="17.875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="19.375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="10.875" style="1"/>
     <col min="22" max="22" width="24.5" style="3" customWidth="1"/>
-    <col min="23" max="23" width="25.1640625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="20.83203125" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="10.83203125" style="1"/>
+    <col min="23" max="23" width="25.125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="20.875" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,25 +779,25 @@
         <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="J2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>22</v>
@@ -794,25 +806,25 @@
         <v>21</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="S2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>2</v>
@@ -821,7 +833,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1001</v>
       </c>
@@ -844,10 +856,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -871,10 +883,10 @@
         <v>11</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S3" s="2">
         <v>1</v>
@@ -886,16 +898,16 @@
         <v>1</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1002</v>
       </c>
@@ -918,10 +930,10 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
@@ -939,10 +951,10 @@
         <v>12</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S4" s="2">
         <v>2</v>
@@ -951,19 +963,19 @@
         <v>6</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1003</v>
       </c>
@@ -986,10 +998,10 @@
         <v>3</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J5" s="2">
         <v>3</v>
@@ -1007,10 +1019,10 @@
         <v>13</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S5" s="2">
         <v>3</v>
@@ -1022,13 +1034,13 @@
         <v>3</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1041,19 +1053,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
     <col min="10" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="20.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1088,10 +1100,10 @@
         <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>100001</v>
       </c>
@@ -1126,10 +1138,10 @@
         <v>15</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100001</v>
       </c>
@@ -1164,10 +1176,10 @@
         <v>15</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1202,10 +1214,10 @@
         <v>15</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100002</v>
       </c>
@@ -1240,10 +1252,10 @@
         <v>15</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100003</v>
       </c>
@@ -1278,11 +1290,12 @@
         <v>15</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1294,71 +1307,71 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: parse timestr with location timezone
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD84106-3BD4-414C-9190-EAEFE63E94A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF85F4D-B348-43F1-8E6C-79EA138BC647}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-435" yWindow="5625" windowWidth="37020" windowHeight="13740" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="4590" yWindow="5580" windowWidth="37020" windowHeight="13740" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="87">
   <si>
     <t>道具ID</t>
   </si>
@@ -282,6 +282,18 @@
   </si>
   <si>
     <t>1h1m1s</t>
+  </si>
+  <si>
+    <t>2020-03-05  05:00:00</t>
+  </si>
+  <si>
+    <t>2020-07-10  05:00:00</t>
+  </si>
+  <si>
+    <t>2020-08-10  05:00:00</t>
+  </si>
+  <si>
+    <t>2020-09-10  05:00:00</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1066,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1147,7 @@
         <v>4</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>79</v>
@@ -1170,10 +1182,10 @@
         <v>2</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>80</v>
@@ -1208,10 +1220,10 @@
         <v>3</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>78</v>
@@ -1246,10 +1258,10 @@
         <v>2</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>82</v>
@@ -1284,7 +1296,7 @@
         <v>2</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
feat: no empty message will be spawned if it is one-level message
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF85F4D-B348-43F1-8E6C-79EA138BC647}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB75B044-D15D-4B74-857E-A253F21907E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="5580" windowWidth="37020" windowHeight="13740" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="1320" yWindow="6330" windowWidth="37020" windowHeight="13740" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
   <si>
     <t>道具ID</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>2020-09-10  05:00:00</t>
+  </si>
+  <si>
+    <t>奖励3ID</t>
+  </si>
+  <si>
+    <t>奖励3NUM</t>
   </si>
 </sst>
 </file>
@@ -668,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3:X5"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1063,21 +1069,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.875" customWidth="1"/>
     <col min="5" max="5" width="23.875" customWidth="1"/>
-    <col min="10" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="20.875" style="1" customWidth="1"/>
+    <col min="12" max="13" width="25" customWidth="1"/>
+    <col min="14" max="14" width="20.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1105,17 +1111,23 @@
       <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>100001</v>
       </c>
@@ -1137,23 +1149,25 @@
       <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="2">
-        <v>2002</v>
-      </c>
-      <c r="I2" s="2">
-        <v>2</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
+        <v>2007</v>
+      </c>
+      <c r="K2" s="2">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100001</v>
       </c>
@@ -1169,119 +1183,109 @@
       <c r="E3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="2">
-        <v>2001</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="2">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="I3" s="2">
         <v>2</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2">
+        <v>2007</v>
+      </c>
+      <c r="K3" s="2">
+        <v>5</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>100001</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="2">
         <v>2002</v>
       </c>
-      <c r="G4" s="2">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2002</v>
-      </c>
-      <c r="I4" s="2">
-        <v>3</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>100002</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2001</v>
-      </c>
       <c r="G5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="2">
         <v>2002</v>
       </c>
       <c r="I5" s="2">
-        <v>2</v>
-      </c>
-      <c r="J5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2002</v>
+      </c>
+      <c r="K5" s="2">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>100003</v>
+        <v>100002</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2">
         <v>2001</v>
@@ -1295,13 +1299,63 @@
       <c r="I6" s="2">
         <v>2</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2">
+        <v>2002</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="N6" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>100003</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2002</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2002</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: empty message check and process related to List and Map
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB75B044-D15D-4B74-857E-A253F21907E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78485C63-30D6-488D-A06A-DD352126E8C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="6330" windowWidth="37020" windowHeight="13740" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="1095" yWindow="3300" windowWidth="37020" windowHeight="13740" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
   <si>
     <t>道具ID</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>奖励3NUM</t>
+  </si>
+  <si>
+    <t>签到活动节3</t>
   </si>
 </sst>
 </file>
@@ -674,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1021,12 +1024,6 @@
       <c r="I5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="2">
-        <v>3</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
       <c r="N5" s="2">
         <v>2002</v>
       </c>
@@ -1069,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1217,119 +1214,107 @@
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2002</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2002</v>
-      </c>
-      <c r="I5" s="2">
-        <v>3</v>
-      </c>
-      <c r="J5" s="2">
-        <v>2002</v>
-      </c>
-      <c r="K5" s="2">
-        <v>3</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>78</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>100002</v>
+        <v>100001</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="G6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2">
         <v>2002</v>
       </c>
       <c r="I6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6" s="2">
         <v>2002</v>
       </c>
       <c r="K6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>100003</v>
+        <v>100002</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="2">
         <v>2001</v>
@@ -1350,12 +1335,56 @@
         <v>2</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>100003</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2002</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2002</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: in-cell composite types
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78485C63-30D6-488D-A06A-DD352126E8C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5056D912-B6A2-4870-9C9D-7FAA32AC62FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="3300" windowWidth="37020" windowHeight="13740" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="4860" yWindow="4500" windowWidth="37020" windowHeight="13740" activeTab="2" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
   <si>
     <t>道具ID</t>
   </si>
@@ -200,9 +200,6 @@
     <t>强化1描述2</t>
   </si>
   <si>
-    <t>强化1描述3</t>
-  </si>
-  <si>
     <t>售卖选项</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>1001:2,1002:5,1003:10</t>
   </si>
   <si>
-    <t>基本信息</t>
-  </si>
-  <si>
     <t>110,标题,内容,true</t>
   </si>
   <si>
@@ -303,6 +297,15 @@
   </si>
   <si>
     <t>签到活动节3</t>
+  </si>
+  <si>
+    <t>基本信息1</t>
+  </si>
+  <si>
+    <t>基本信息2</t>
+  </si>
+  <si>
+    <t>220,标题2</t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -708,76 +711,76 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -809,16 +812,16 @@
         <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>22</v>
@@ -836,16 +839,16 @@
         <v>48</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>2</v>
@@ -919,13 +922,13 @@
         <v>1</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -987,13 +990,13 @@
         <v>46</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1009,21 +1012,6 @@
       <c r="D5" s="1">
         <v>5001003</v>
       </c>
-      <c r="E5" s="2">
-        <v>2001</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <v>3</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="N5" s="2">
         <v>2002</v>
       </c>
@@ -1049,13 +1037,13 @@
         <v>3</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1068,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -1109,10 +1097,10 @@
         <v>24</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>13</v>
@@ -1158,10 +1146,10 @@
         <v>4</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1195,13 +1183,13 @@
         <v>5</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1218,7 +1206,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1227,13 +1215,13 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1291,13 +1279,13 @@
         <v>3</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1335,13 +1323,13 @@
         <v>2</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1379,13 +1367,13 @@
         <v>2</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1396,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788C4DC7-4113-0642-9BB8-FA63AD1AD680}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1398,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
@@ -1418,7 +1406,7 @@
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
@@ -1426,7 +1414,7 @@
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -1437,36 +1425,44 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>68</v>
+        <v>89</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: generator: proto -> xlsx
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5056D912-B6A2-4870-9C9D-7FAA32AC62FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3783EAF4-B6ED-4616-88B5-5D423189379F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="4500" windowWidth="37020" windowHeight="13740" activeTab="2" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="735" yWindow="5235" windowWidth="37020" windowHeight="13740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -702,8 +702,8 @@
     <col min="18" max="18" width="19.625" style="2" customWidth="1"/>
     <col min="19" max="19" width="17.875" style="2" customWidth="1"/>
     <col min="20" max="20" width="19.375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="10.875" style="1"/>
-    <col min="22" max="22" width="24.5" style="3" customWidth="1"/>
+    <col min="21" max="21" width="24.5" style="3" customWidth="1"/>
+    <col min="22" max="22" width="10.875" style="1"/>
     <col min="23" max="23" width="25.125" style="3" customWidth="1"/>
     <col min="24" max="24" width="20.875" style="1" customWidth="1"/>
     <col min="25" max="16384" width="10.875" style="1"/>
@@ -844,11 +844,11 @@
       <c r="T2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>2</v>
@@ -918,11 +918,11 @@
       <c r="T3" s="2">
         <v>5</v>
       </c>
-      <c r="U3" s="1">
-        <v>1</v>
-      </c>
-      <c r="V3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>57</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>4</v>
@@ -986,11 +986,11 @@
       <c r="T4" s="2">
         <v>6</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>4</v>
@@ -1033,11 +1033,11 @@
       <c r="T5" s="2">
         <v>7</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="W5" s="3" t="s">
         <v>4</v>
@@ -1386,7 +1386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788C4DC7-4113-0642-9BB8-FA63AD1AD680}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: allow newline in caption for clear representation of nested types
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Github/tableau/cmd/test/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3783EAF4-B6ED-4616-88B5-5D423189379F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80369AB9-4432-A54C-9663-6AD8E74F29B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="5235" windowWidth="37020" windowHeight="13740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>游戏内稀有货币</t>
   </si>
   <si>
-    <t>属性1ID</t>
-  </si>
-  <si>
     <t>属性2Value</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>奖励1NUM</t>
   </si>
   <si>
-    <t>属性1Value</t>
-  </si>
-  <si>
     <t>章描述</t>
   </si>
   <si>
@@ -155,15 +149,6 @@
     <t>持续多久</t>
   </si>
   <si>
-    <t>属性1强化1ID</t>
-  </si>
-  <si>
-    <t>属性1强化1描述</t>
-  </si>
-  <si>
-    <t>属性1强化1提示列表</t>
-  </si>
-  <si>
     <t>新,热,限</t>
   </si>
   <si>
@@ -242,18 +227,6 @@
     <t>15.246879</t>
   </si>
   <si>
-    <t>属性1抑制1类型</t>
-  </si>
-  <si>
-    <t>属性1抑制1数量</t>
-  </si>
-  <si>
-    <t>属性1抑制2类型</t>
-  </si>
-  <si>
-    <t>属性1抑制2数量</t>
-  </si>
-  <si>
     <t>属性2抑制1类型</t>
   </si>
   <si>
@@ -306,6 +279,49 @@
   </si>
   <si>
     <t>220,标题2</t>
+  </si>
+  <si>
+    <t>属性1
+Value</t>
+  </si>
+  <si>
+    <t>属性1
+强化1
+ID</t>
+  </si>
+  <si>
+    <t>属性1
+强化1
+描述</t>
+  </si>
+  <si>
+    <t>属性1
+强化1
+提示列表</t>
+  </si>
+  <si>
+    <t>属性1
+抑制1
+类型</t>
+  </si>
+  <si>
+    <t>属性1
+抑制1
+数量</t>
+  </si>
+  <si>
+    <t>属性1
+抑制2
+类型</t>
+  </si>
+  <si>
+    <t>属性1
+抑制2
+数量</t>
+  </si>
+  <si>
+    <t>属性1
+ID</t>
   </si>
 </sst>
 </file>
@@ -321,7 +337,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +347,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,9 +386,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -382,7 +413,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -681,183 +712,183 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.875" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="1"/>
-    <col min="5" max="5" width="10.875" style="2"/>
-    <col min="6" max="8" width="14.375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="18.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="8" width="14.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="18.5" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.875" style="2"/>
+    <col min="14" max="14" width="10.83203125" style="2"/>
     <col min="15" max="15" width="12.5" style="2" customWidth="1"/>
-    <col min="16" max="17" width="14.375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="19.625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="17.875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="19.375" style="2" customWidth="1"/>
+    <col min="16" max="17" width="14.33203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.6640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="17.83203125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" style="2" customWidth="1"/>
     <col min="21" max="21" width="24.5" style="3" customWidth="1"/>
-    <col min="22" max="22" width="10.875" style="1"/>
-    <col min="23" max="23" width="25.125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="20.875" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="10.875" style="1"/>
+    <col min="22" max="22" width="10.83203125" style="1"/>
+    <col min="23" max="23" width="25.1640625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="20.83203125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="P2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="R2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1001</v>
       </c>
@@ -880,10 +911,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -907,10 +938,10 @@
         <v>11</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="S3" s="2">
         <v>1</v>
@@ -919,7 +950,7 @@
         <v>5</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="V3" s="1">
         <v>1</v>
@@ -928,10 +959,10 @@
         <v>4</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1002</v>
       </c>
@@ -954,10 +985,10 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
@@ -975,10 +1006,10 @@
         <v>12</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="S4" s="2">
         <v>2</v>
@@ -987,19 +1018,19 @@
         <v>6</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1003</v>
       </c>
@@ -1022,10 +1053,10 @@
         <v>13</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="S5" s="2">
         <v>3</v>
@@ -1034,7 +1065,7 @@
         <v>7</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>3</v>
@@ -1043,7 +1074,7 @@
         <v>4</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1060,15 +1091,15 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
     <col min="12" max="13" width="25" customWidth="1"/>
-    <col min="14" max="14" width="20.875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1076,31 +1107,31 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>13</v>
@@ -1109,10 +1140,10 @@
         <v>14</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>100001</v>
       </c>
@@ -1120,13 +1151,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2">
         <v>2001</v>
@@ -1146,13 +1177,13 @@
         <v>4</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>100001</v>
       </c>
@@ -1160,13 +1191,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1183,16 +1214,16 @@
         <v>5</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1200,13 +1231,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1215,16 +1246,16 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1232,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1244,7 +1275,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1252,13 +1283,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="2">
         <v>2002</v>
@@ -1279,16 +1310,16 @@
         <v>3</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>100002</v>
       </c>
@@ -1296,13 +1327,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2">
         <v>2001</v>
@@ -1323,16 +1354,16 @@
         <v>2</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>100003</v>
       </c>
@@ -1340,13 +1371,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2">
         <v>2001</v>
@@ -1367,13 +1398,13 @@
         <v>2</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1390,79 +1421,79 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: default settings for map 'key' and list 'name'
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Github/tableau/cmd/test/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80369AB9-4432-A54C-9663-6AD8E74F29B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72E4CBC-FF87-4291-B047-6B5A5B979A36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="3015" yWindow="2490" windowWidth="32040" windowHeight="16995" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
     <sheet name="Activity" sheetId="2" r:id="rId2"/>
     <sheet name="Env" sheetId="3" r:id="rId3"/>
+    <sheet name="Mail" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="102">
   <si>
     <t>道具ID</t>
   </si>
@@ -101,18 +102,6 @@
     <t>属性2ID</t>
   </si>
   <si>
-    <t>奖励1ID</t>
-  </si>
-  <si>
-    <t>奖励2NUM</t>
-  </si>
-  <si>
-    <t>奖励2ID</t>
-  </si>
-  <si>
-    <t>奖励1NUM</t>
-  </si>
-  <si>
     <t>章描述</t>
   </si>
   <si>
@@ -261,12 +250,6 @@
   </si>
   <si>
     <t>2020-09-10  05:00:00</t>
-  </si>
-  <si>
-    <t>奖励3ID</t>
-  </si>
-  <si>
-    <t>奖励3NUM</t>
   </si>
   <si>
     <t>签到活动节3</t>
@@ -322,6 +305,57 @@
   <si>
     <t>属性1
 ID</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>开服奖励</t>
+  </si>
+  <si>
+    <t>中秋福利</t>
+  </si>
+  <si>
+    <t>开服啦，大波福利送给你！</t>
+  </si>
+  <si>
+    <t>中秋佳节，与你相伴！</t>
+  </si>
+  <si>
+    <t>Item1Num</t>
+  </si>
+  <si>
+    <t>Item2Num</t>
+  </si>
+  <si>
+    <t>Item1Id</t>
+  </si>
+  <si>
+    <t>Item2Id</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>奖励1Num</t>
+  </si>
+  <si>
+    <t>奖励2Num</t>
+  </si>
+  <si>
+    <t>奖励3Num</t>
+  </si>
+  <si>
+    <t>奖励1Id</t>
+  </si>
+  <si>
+    <t>奖励2Id</t>
+  </si>
+  <si>
+    <t>奖励3Id</t>
+  </si>
+  <si>
+    <t>Key</t>
   </si>
 </sst>
 </file>
@@ -397,7 +431,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,7 +447,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -711,110 +745,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.875" style="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="8" width="14.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="1"/>
+    <col min="5" max="5" width="10.875" style="2"/>
+    <col min="6" max="8" width="14.375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="18.625" style="2" customWidth="1"/>
     <col min="13" max="13" width="18.5" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="10.875" style="2"/>
     <col min="15" max="15" width="12.5" style="2" customWidth="1"/>
-    <col min="16" max="17" width="14.33203125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="17.83203125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" style="2" customWidth="1"/>
+    <col min="16" max="17" width="14.375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="17.875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="19.375" style="2" customWidth="1"/>
     <col min="21" max="21" width="24.5" style="3" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" style="1"/>
-    <col min="23" max="23" width="25.1640625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="20.83203125" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="10.83203125" style="1"/>
+    <col min="22" max="22" width="10.875" style="1"/>
+    <col min="23" max="23" width="25.125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="20.875" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -828,31 +862,31 @@
         <v>6</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>21</v>
@@ -861,22 +895,22 @@
         <v>20</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="V2" s="6" t="s">
         <v>9</v>
@@ -885,10 +919,10 @@
         <v>2</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1001</v>
       </c>
@@ -911,10 +945,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -938,10 +972,10 @@
         <v>11</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S3" s="2">
         <v>1</v>
@@ -950,7 +984,7 @@
         <v>5</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="V3" s="1">
         <v>1</v>
@@ -959,10 +993,10 @@
         <v>4</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1002</v>
       </c>
@@ -985,10 +1019,10 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
@@ -1006,10 +1040,10 @@
         <v>12</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="S4" s="2">
         <v>2</v>
@@ -1018,19 +1052,19 @@
         <v>6</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1003</v>
       </c>
@@ -1053,10 +1087,10 @@
         <v>13</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="S5" s="2">
         <v>3</v>
@@ -1065,7 +1099,7 @@
         <v>7</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>3</v>
@@ -1074,7 +1108,7 @@
         <v>4</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1088,18 +1122,18 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
     <col min="12" max="13" width="25" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1107,31 +1141,31 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>13</v>
@@ -1140,10 +1174,10 @@
         <v>14</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>100001</v>
       </c>
@@ -1151,13 +1185,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2">
         <v>2001</v>
@@ -1177,13 +1211,13 @@
         <v>4</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100001</v>
       </c>
@@ -1191,13 +1225,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1214,16 +1248,16 @@
         <v>5</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1231,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1246,16 +1280,16 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1263,7 +1297,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1275,7 +1309,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1283,13 +1317,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2">
         <v>2002</v>
@@ -1310,16 +1344,16 @@
         <v>3</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100002</v>
       </c>
@@ -1327,13 +1361,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7" s="2">
         <v>2001</v>
@@ -1354,16 +1388,16 @@
         <v>2</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100003</v>
       </c>
@@ -1371,13 +1405,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2">
         <v>2001</v>
@@ -1398,13 +1432,13 @@
         <v>2</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1418,82 +1452,173 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>63</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9028F340-E511-4441-B0B2-3776D1CB0FD8}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2">
+        <v>1001</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>1002</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3">
+        <v>2001</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>2002</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: protoconf proposal and xlsxgen
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72E4CBC-FF87-4291-B047-6B5A5B979A36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD4DB8A-2FC3-4C95-B155-FFF66BEBDCB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="2490" windowWidth="32040" windowHeight="16995" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-990" yWindow="4755" windowWidth="32040" windowHeight="16995" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1539,7 +1539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9028F340-E511-4441-B0B2-3776D1CB0FD8}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: support struct with fields spanning multiple columns
</commit_message>
<xml_diff>
--- a/cmd/test/testdata/Test.xlsx
+++ b/cmd/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\cmd\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD4DB8A-2FC3-4C95-B155-FFF66BEBDCB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03EF416-973A-46A0-AC34-DFF61631E760}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-990" yWindow="4755" windowWidth="32040" windowHeight="16995" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-39120" yWindow="11070" windowWidth="44280" windowHeight="13800" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>道具ID</t>
   </si>
@@ -356,6 +356,15 @@
   </si>
   <si>
     <t>Key</t>
+  </si>
+  <si>
+    <t>任务类型</t>
+  </si>
+  <si>
+    <t>任务目标</t>
+  </si>
+  <si>
+    <t>任务参数</t>
   </si>
 </sst>
 </file>
@@ -745,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1119,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1133,7 +1142,7 @@
     <col min="14" max="14" width="20.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1176,8 +1185,17 @@
       <c r="N1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>100001</v>
       </c>
@@ -1216,8 +1234,17 @@
       <c r="N2" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100001</v>
       </c>
@@ -1256,8 +1283,17 @@
       <c r="N3" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1288,8 +1324,17 @@
       <c r="N4" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1309,7 +1354,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1352,8 +1397,17 @@
       <c r="N6" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="1">
+        <v>2</v>
+      </c>
+      <c r="P6" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100002</v>
       </c>
@@ -1396,8 +1450,17 @@
       <c r="N7" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="1">
+        <v>2</v>
+      </c>
+      <c r="P7" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100003</v>
       </c>
@@ -1439,6 +1502,15 @@
       </c>
       <c r="N8" s="3" t="s">
         <v>66</v>
+      </c>
+      <c r="O8" s="1">
+        <v>2</v>
+      </c>
+      <c r="P8" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>